<commit_message>
data scraping, write to excel, upload to Google Drive, nu merge Gmail
</commit_message>
<xml_diff>
--- a/SteamGameFinder/games_to_find1.xlsx
+++ b/SteamGameFinder/games_to_find1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1190B7-46C0-43AD-A5AD-C3A461859A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863B22F5-3283-45B8-A389-B1A82EB5DB29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3030" windowWidth="28800" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3375" yWindow="3375" windowWidth="28800" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -56,6 +56,15 @@
   </si>
   <si>
     <t>a_diana_gherghescu@yahoo.com</t>
+  </si>
+  <si>
+    <t>David Bejenariu</t>
+  </si>
+  <si>
+    <t>david.bejenariu@gmail.com</t>
+  </si>
+  <si>
+    <t>Black</t>
   </si>
 </sst>
 </file>
@@ -384,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,10 +448,25 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{56277BB1-1D91-4347-A294-47C2867BCDB3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>